<commit_message>
Manual Test Case - Minor Changes Updated
</commit_message>
<xml_diff>
--- a/project-mgmt/design/Testing/Manual Test/CHHS_Mannual_TestCases_1st June.xlsx
+++ b/project-mgmt/design/Testing/Manual Test/CHHS_Mannual_TestCases_1st June.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek.m\Desktop\CHHS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul.bhaskar\Documents\GitHub\demo\project-mgmt\design\Testing\Manual Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -456,208 +456,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> URL.
-2. Check wether header tab </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">About Us </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is clickable or not.
-3  Check wether header tab </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>For Families</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is clickable or not.
-4. Check wether header tab T</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aining</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is clickable or not.
-5. Check wether header tab </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Contct Us</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is clickable or not.
-6. Check wether header tab </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Search</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is clickable or not.
-7. Check wether header tab </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Login</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is clickable or not.
-8. Check wether header tab </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Help</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is clickable or not.
-9. Check wether </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Family Registration</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> link is clickable or not.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Open the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CHHS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> URL.
 2. Click on</t>
     </r>
     <r>
@@ -2629,13 +2427,215 @@
         <scheme val="minor"/>
       </rPr>
       <t>Button to Cancel.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Open the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CHHS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> URL.
+2. Check whether header tab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">About Us </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is clickable or not.
+3  Check whether header tab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For Families</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is clickable or not.
+4. Check whether header tab T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ainting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is clickable or not.
+5. Check whether header tab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Contact Us</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is clickable or not.
+6. Check whether header tab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is clickable or not.
+7. Check whether header tab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is clickable or not.
+8. Check whether header tab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Help</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is clickable or not.
+9. Check whether </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Family Registration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> link is clickable or not.</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3095,7 +3095,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,7 +3166,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>10</v>
@@ -3217,7 +3217,7 @@
         <v>42522</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
@@ -3226,7 +3226,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>24</v>
@@ -3247,7 +3247,7 @@
         <v>42522</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
@@ -3256,7 +3256,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>25</v>
@@ -3277,7 +3277,7 @@
         <v>42522</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>20</v>
@@ -3286,7 +3286,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>26</v>
@@ -3316,7 +3316,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>27</v>
@@ -3337,7 +3337,7 @@
         <v>42522</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>22</v>
@@ -3346,7 +3346,7 @@
         <v>9</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>28</v>
@@ -3367,7 +3367,7 @@
         <v>42522</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="str">
         <f>I4</f>

</xml_diff>

<commit_message>
Manual Test Case - Minor Changes - Updated
</commit_message>
<xml_diff>
--- a/project-mgmt/design/Testing/Manual Test/CHHS_Mannual_TestCases_1st June.xlsx
+++ b/project-mgmt/design/Testing/Manual Test/CHHS_Mannual_TestCases_1st June.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="2" r:id="rId1"/>
+    <sheet name="CHHS-TC" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <t>TC ID</t>
   </si>
@@ -50,9 +51,6 @@
     <t>Expected Result</t>
   </si>
   <si>
-    <t>Actual Behaviour</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -114,9 +112,6 @@
   </si>
   <si>
     <t>user should be able to post query on the portal successfully</t>
-  </si>
-  <si>
-    <t>To Verify the all the lebels and linkes present on home page</t>
   </si>
   <si>
     <r>
@@ -2630,13 +2625,122 @@
       </rPr>
       <t xml:space="preserve"> link is clickable or not.</t>
     </r>
+  </si>
+  <si>
+    <t>To Verify the all the labels and links present on home page</t>
+  </si>
+  <si>
+    <t>Actual Behavior</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>CHHS_TC1</t>
+  </si>
+  <si>
+    <t>CHHS_TC2</t>
+  </si>
+  <si>
+    <t>CHHS_TC3</t>
+  </si>
+  <si>
+    <t>BRD Req #</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>UC_3.2</t>
+  </si>
+  <si>
+    <t>CHHS_TC4</t>
+  </si>
+  <si>
+    <t>CHHS_TC5</t>
+  </si>
+  <si>
+    <t>CHHS_TC6</t>
+  </si>
+  <si>
+    <t>CHHS_TC7</t>
+  </si>
+  <si>
+    <t>UC_3.3</t>
+  </si>
+  <si>
+    <t>UC_3.1</t>
+  </si>
+  <si>
+    <t>UC_3.4</t>
+  </si>
+  <si>
+    <t>Document Information</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Reviewers</t>
+  </si>
+  <si>
+    <t>Amit Sikka</t>
+  </si>
+  <si>
+    <t>Ver 1.0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Revision History of Test Plan </t>
+    </r>
+  </si>
+  <si>
+    <t>Description/Change</t>
+  </si>
+  <si>
+    <t>Prepared/Modified By</t>
+  </si>
+  <si>
+    <t>Reviewed by</t>
+  </si>
+  <si>
+    <t>Date of review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Approved By</t>
+  </si>
+  <si>
+    <t>Approved Date</t>
+  </si>
+  <si>
+    <t>Initial Draft</t>
+  </si>
+  <si>
+    <t>Vivek Kumar Mishra</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2681,8 +2785,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2701,8 +2820,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2779,11 +2910,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2810,6 +3015,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3091,29 +3333,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="B3:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="19.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="9" customWidth="1"/>
+    <col min="5" max="8" width="14.140625" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="16">
+        <v>42522</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="16">
+        <v>42522</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="28" style="9" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.140625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="8"/>
+    <col min="3" max="4" width="11.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="28" style="9" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="63.140625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3121,269 +3511,321 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>8</v>
+      <c r="L1" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="7">
         <v>42522</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="7">
+        <v>42522</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="7">
-        <v>42522</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>11</v>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="390" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="7">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="7">
         <v>42522</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>11</v>
+      <c r="G4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="7">
+      <c r="D5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="7">
         <v>42522</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>11</v>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="7">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="7">
         <v>42522</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>11</v>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="7">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="7">
         <v>42522</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="7">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7">
         <v>42522</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>11</v>
+      <c r="G8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="7">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="7">
         <v>42522</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="3" t="str">
-        <f>I4</f>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f>K4</f>
         <v>Use should be able to manage his profile without any abnormal behaviour of portal.</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>11</v>
+      <c r="I9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>